<commit_message>
everything working as intended for now
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -14,90 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>URL</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202302204461549?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202306058163586?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202405139652007?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202407011312408?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202409204270639?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202410084967287?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202410295706788?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202410295712702?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202411015835018?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202411146282450?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
   </si>
   <si>
     <t>https://www.autotrader.co.uk/car-details/202411156319287?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
   </si>
   <si>
-    <t>https://www.autotrader.co.uk/car-details/202412036942163?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202412077088745?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202412317639076?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202501158046351?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202501188152626?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202501308577450?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202502018634758?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202502038698884?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202502078873648?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202502199256509?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202502219353755?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202502229382614?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202502259476344?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202503029658728?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202503039693826?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
-  </si>
-  <si>
-    <t>https://www.autotrader.co.uk/car-details/202503019623450?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+    <t>https://www.autotrader.co.uk/car-details/202411146282450?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
   </si>
 </sst>
 </file>
@@ -468,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A28"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -489,160 +414,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-    <hyperlink ref="A7" r:id="rId6"/>
-    <hyperlink ref="A8" r:id="rId7"/>
-    <hyperlink ref="A9" r:id="rId8"/>
-    <hyperlink ref="A10" r:id="rId9"/>
-    <hyperlink ref="A11" r:id="rId10"/>
-    <hyperlink ref="A12" r:id="rId11"/>
-    <hyperlink ref="A13" r:id="rId12"/>
-    <hyperlink ref="A14" r:id="rId13"/>
-    <hyperlink ref="A15" r:id="rId14"/>
-    <hyperlink ref="A16" r:id="rId15"/>
-    <hyperlink ref="A17" r:id="rId16"/>
-    <hyperlink ref="A18" r:id="rId17"/>
-    <hyperlink ref="A19" r:id="rId18"/>
-    <hyperlink ref="A20" r:id="rId19"/>
-    <hyperlink ref="A21" r:id="rId20"/>
-    <hyperlink ref="A22" r:id="rId21"/>
-    <hyperlink ref="A23" r:id="rId22"/>
-    <hyperlink ref="A24" r:id="rId23"/>
-    <hyperlink ref="A25" r:id="rId24"/>
-    <hyperlink ref="A26" r:id="rId25"/>
-    <hyperlink ref="A27" r:id="rId26"/>
-    <hyperlink ref="A28" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EVERYTHING FINALLY WORKS AS INTENDED...FOR NOW
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -1,35 +1,131 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Coding Projects\autotrader-tracker\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAA29D5-D184-4ACC-AE6D-ABA7C32131D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>URL</t>
   </si>
   <si>
+    <t>https://www.autotrader.co.uk/car-details/202302204461549?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202306058163586?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202405139652007?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202407011312408?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202409204270639?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202410084967287?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202410295706788?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202410295712702?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202411015835018?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202411146282450?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
     <t>https://www.autotrader.co.uk/car-details/202411156319287?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
   </si>
   <si>
-    <t>https://www.autotrader.co.uk/car-details/202411146282450?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+    <t>https://www.autotrader.co.uk/car-details/202412036942163?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202412077088745?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202412317639076?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202501158046351?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202501188152626?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202501308577450?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202502018634758?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202502038698884?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202502078873648?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202502199256509?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202502219353755?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202502229382614?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202502259476344?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202503029658728?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202503039693826?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202503019623450?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202503049742784?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202503079858704?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202503059791560?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202503049732509?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
+  </si>
+  <si>
+    <t>https://www.autotrader.co.uk/car-details/202503059777856?fromSavedAds=true&amp;advertising-location=at_cars&amp;sort=relevance&amp;postcode=CB58TJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,13 +201,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -149,7 +253,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -183,6 +287,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -217,9 +322,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -392,32 +498,209 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>